<commit_message>
Added tables to manuscript
</commit_message>
<xml_diff>
--- a/Manuscript/Tables/Table2-SurfaceComplRxns.xlsx
+++ b/Manuscript/Tables/Table2-SurfaceComplRxns.xlsx
@@ -494,16 +494,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="44.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="44.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="52.25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="52.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -925,7 +925,7 @@
       <c r="B45">
         <v>0</v>
       </c>
-      <c r="C45">
+      <c r="C45" s="1">
         <f>0.000000006/0.03</f>
         <v>2.0000000000000002E-7</v>
       </c>
@@ -950,5 +950,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>